<commit_message>
excel reading in pandas updated to dynamic
</commit_message>
<xml_diff>
--- a/Capstone Excel report format.xlsx
+++ b/Capstone Excel report format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMoreira\Class Projects\Capstone\Cookie-Quest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFD79F6-3A96-42D3-ABA4-C6B10CA86FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB645AF-7816-4105-B965-141EF81728DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC594F40-63CB-4CE1-BF75-B047599128FD}"/>
+    <workbookView xWindow="5415" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{AC594F40-63CB-4CE1-BF75-B047599128FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>CCM Implemented</t>
   </si>
@@ -146,10 +146,40 @@
     <t>aga-us.com</t>
   </si>
   <si>
-    <t>www.facebook.com</t>
-  </si>
-  <si>
-    <t>www.instagram.com</t>
+    <t>https://ironwoodins.com/</t>
+  </si>
+  <si>
+    <t>https://icip.marshpm.com/FedExWeb/</t>
+  </si>
+  <si>
+    <t>https://www.marshmanagement.com/</t>
+  </si>
+  <si>
+    <t>https://www.linqbymarsh.com/blueicyber/</t>
+  </si>
+  <si>
+    <t>https://services.marshspecialty.com/msp-web/register?division=MSP&amp;client=SF</t>
+  </si>
+  <si>
+    <t>https://www.dovetailexchange.com/Account/Login</t>
+  </si>
+  <si>
+    <t>http://victorinsurance.it/</t>
+  </si>
+  <si>
+    <t>https://www.sanint.it/</t>
+  </si>
+  <si>
+    <t>http://www.victorinsurance.nl/</t>
+  </si>
+  <si>
+    <t>https://marshwritingsubmissioncenter.com</t>
+  </si>
+  <si>
+    <t>https://nordicportal.marsh.com/dk/crm/crm_internet.nsf?login</t>
+  </si>
+  <si>
+    <t>https://victorinsurance.nl/verzekeraars/</t>
   </si>
 </sst>
 </file>
@@ -224,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,6 +266,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -551,15 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931DABA6-9C1C-439A-A1CA-07FC3B7AEEF2}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -596,160 +630,307 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="45">
+      <c r="A6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
-        <v>22</v>
+      <c r="A16" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
+      <c r="A20" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="5" t="s">
-        <v>27</v>
+      <c r="A21" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="3" t="s">
-        <v>33</v>
+      <c r="A27" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="6" t="s">
-        <v>37</v>
-      </c>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A30" r:id="rId1" xr:uid="{4CA8AD5D-2410-4915-8AD7-BE87BECBB2C5}"/>
-    <hyperlink ref="A31" r:id="rId2" xr:uid="{96A997DF-1490-4B6A-BFF2-DFB99ECB9222}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6F4F8581-92C3-4E37-AC70-FFAE43AF617D}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{876E3286-722D-41E5-B927-E8EAE16E5588}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{860CDBE1-63B1-4D73-95B2-2B11418DD2B6}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{2DA23B16-3F7A-4F9A-9992-3BC72ABDEA36}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{D555A742-759C-4D27-8C3E-2ED3DABFF21D}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{F51B34FD-BE34-449F-8674-D3BDE84DDE2A}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{AD3B3C3D-2317-42C6-8126-7A846FD53FDC}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{A6F23ABB-422F-4E0A-AED3-C8DDFEB4C2DF}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{862CB241-BD77-44C5-B74B-379017A320C2}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{D1A84C52-DC93-4EAA-9A7B-1D4511EE7969}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{02770B0E-6132-4980-93F3-D8F5039F716D}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{F2D4627C-0066-4D5B-A538-EC69A906B255}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>